<commit_message>
Cập Nhật Dữ Liệu Mẫu
</commit_message>
<xml_diff>
--- a/WebsiteTinTuc/Dữ Liệu Tin Tức.xlsx
+++ b/WebsiteTinTuc/Dữ Liệu Tin Tức.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NLU\Nam 3\CongNghePhanMiem\GK L1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NLU\Nam 3\CongNghePhanMiem\GK L1\CNPM08\WebsiteTinTuc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EE2E6B-B666-4260-ADD9-EF0AE9887B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9A36C-1EAD-4F1F-BB87-0FB9C5C118EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Article" sheetId="1" r:id="rId1"/>
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -999,10 +999,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>147</v>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="H2" s="6">
         <f ca="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44704</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="71.25">
@@ -1057,11 +1057,11 @@
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G21" ca="1" si="0">CHOOSE(RANDBETWEEN(1,3),"Minh Chánh","Phát Đạt","Quốc Nghĩa")</f>
-        <v>Phát Đạt</v>
+        <v>Minh Chánh</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" ref="H3:H21" ca="1" si="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44617</v>
+        <v>44604</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="199.5">
@@ -1085,11 +1085,11 @@
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>Quốc Nghĩa</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44569</v>
+        <v>44690</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="85.5">
@@ -1113,11 +1113,11 @@
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>Quốc Nghĩa</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44682</v>
+        <v>44665</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="85.5">
@@ -1141,11 +1141,11 @@
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>Quốc Nghĩa</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44693</v>
+        <v>44586</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="313.5">
@@ -1169,11 +1169,11 @@
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>Minh Chánh</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44714</v>
+        <v>44613</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="162" customHeight="1">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="H8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44624</v>
+        <v>44583</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="242.25">
@@ -1225,11 +1225,11 @@
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>Minh Chánh</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44736</v>
+        <v>44710</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="213.75">
@@ -1253,11 +1253,11 @@
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>Phát Đạt</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44718</v>
+        <v>44563</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="171">
@@ -1281,11 +1281,11 @@
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>Quốc Nghĩa</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44578</v>
+        <v>44682</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="213.75">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>Phát Đạt</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44667</v>
+        <v>44733</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="256.5">
@@ -1337,11 +1337,11 @@
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>Phát Đạt</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44717</v>
+        <v>44674</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="256.5">
@@ -1365,11 +1365,11 @@
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>Quốc Nghĩa</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44700</v>
+        <v>44592</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="213.75">
@@ -1393,11 +1393,11 @@
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>Quốc Nghĩa</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44657</v>
+        <v>44684</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="242.25">
@@ -1421,11 +1421,11 @@
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>Quốc Nghĩa</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44606</v>
+        <v>44717</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="228">
@@ -1449,11 +1449,11 @@
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>Minh Chánh</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44676</v>
+        <v>44719</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="165">
@@ -1477,11 +1477,11 @@
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>Minh Chánh</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44684</v>
+        <v>44733</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="185.25">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="H19" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44717</v>
+        <v>44563</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="270.75">
@@ -1533,11 +1533,11 @@
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>Minh Chánh</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44611</v>
+        <v>44652</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="228">
@@ -1561,11 +1561,11 @@
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>Phát Đạt</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44720</v>
+        <v>44607</v>
       </c>
     </row>
   </sheetData>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="C2" s="8">
         <f ca="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44731</v>
+        <v>44685</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="C3" s="8">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44694</v>
+        <v>44658</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="C4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44671</v>
+        <v>44567</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="C5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44712</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="C6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44632</v>
+        <v>44698</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="C7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44703</v>
+        <v>44595</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="C8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44643</v>
+        <v>44566</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="H2" s="8">
         <f ca="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44610</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="H3" s="8">
         <f t="shared" ref="H3:H6" ca="1" si="0">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44632</v>
+        <v>44726</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="H4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44682</v>
+        <v>44599</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="H5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44647</v>
+        <v>44634</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="H6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44723</v>
+        <v>44743</v>
       </c>
     </row>
   </sheetData>
@@ -1880,7 +1880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5458866-346D-4D8E-9E2A-A3385C004668}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sửa dữ liệu mẫu, code tìm kiếm
</commit_message>
<xml_diff>
--- a/WebsiteTinTuc/Dữ Liệu Tin Tức.xlsx
+++ b/WebsiteTinTuc/Dữ Liệu Tin Tức.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NLU\Nam 3\CongNghePhanMiem\GK L1\CNPM08\WebsiteTinTuc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9A36C-1EAD-4F1F-BB87-0FB9C5C118EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2134217A-7D0A-4F9D-89B3-E96ECE61B027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Article" sheetId="1" r:id="rId1"/>
     <sheet name="Type" sheetId="2" r:id="rId2"/>
-    <sheet name="Author" sheetId="3" r:id="rId3"/>
-    <sheet name="Customer" sheetId="4" r:id="rId4"/>
+    <sheet name="User" sheetId="4" r:id="rId3"/>
+    <sheet name="Decentralization" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="154">
   <si>
     <t>id</t>
   </si>
@@ -65,72 +65,6 @@
   </si>
   <si>
     <t>Theo Hãng tin Reuters, trong email gửi tới trưởng các bộ phận trong ngày 2-6, ông Musk đã nêu những lo ngại của mình và yêu cầu họ "tạm dừng tất cả việc tuyển dụng trên toàn cầu".</t>
-  </si>
-  <si>
-    <t>AI_01</t>
-  </si>
-  <si>
-    <t>hongvan@gmail.com</t>
-  </si>
-  <si>
-    <t>AI_02</t>
-  </si>
-  <si>
-    <t>AI_03</t>
-  </si>
-  <si>
-    <t>AI_04</t>
-  </si>
-  <si>
-    <t>AI_05</t>
-  </si>
-  <si>
-    <t>Hồng Vân</t>
-  </si>
-  <si>
-    <t>Minh Chánh</t>
-  </si>
-  <si>
-    <t>Minh Châu</t>
-  </si>
-  <si>
-    <t>Phát Đạt</t>
-  </si>
-  <si>
-    <t>Quốc Nghĩa</t>
-  </si>
-  <si>
-    <t>minhchanh@gmail.com</t>
-  </si>
-  <si>
-    <t>minhchau@gmail.com</t>
-  </si>
-  <si>
-    <t>phatdat@gmail.com</t>
-  </si>
-  <si>
-    <t>quocnghia@gmail.com</t>
-  </si>
-  <si>
-    <t>T_01</t>
-  </si>
-  <si>
-    <t>T_02</t>
-  </si>
-  <si>
-    <t>T_03</t>
-  </si>
-  <si>
-    <t>T_04</t>
-  </si>
-  <si>
-    <t>T_05</t>
-  </si>
-  <si>
-    <t>T_06</t>
-  </si>
-  <si>
-    <t>T_07</t>
   </si>
   <si>
     <t>https://cdn.tuoitre.vn/thumb_w/586/2022/6/4/2022-06-01t144516z1186484414rc21ju9ik9icrtrmadp3health-coronavirus-tesla-16543136074731964354828.jpg</t>
@@ -213,27 +147,6 @@
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>hongvan</t>
-  </si>
-  <si>
-    <t>minhchanh</t>
-  </si>
-  <si>
-    <t>minhchau</t>
-  </si>
-  <si>
-    <t>phatdat</t>
-  </si>
-  <si>
-    <t>quocnghia</t>
-  </si>
-  <si>
-    <t>author_name</t>
-  </si>
-  <si>
-    <t>type_name</t>
   </si>
   <si>
     <t>A_06</t>
@@ -571,13 +484,103 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>Lê</t>
-  </si>
-  <si>
-    <t>Nguyễn Võ</t>
-  </si>
-  <si>
     <t>phone</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>U01</t>
+  </si>
+  <si>
+    <t>U02</t>
+  </si>
+  <si>
+    <t>U03</t>
+  </si>
+  <si>
+    <t>U04</t>
+  </si>
+  <si>
+    <t>u546123</t>
+  </si>
+  <si>
+    <t>u546124</t>
+  </si>
+  <si>
+    <t>u546125</t>
+  </si>
+  <si>
+    <t>u546126</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>Minh Chanh</t>
+  </si>
+  <si>
+    <t>Viet Cuong</t>
+  </si>
+  <si>
+    <t>Hoang Nguyen</t>
+  </si>
+  <si>
+    <t>Nguyen Vo</t>
+  </si>
+  <si>
+    <t>Phat Dat</t>
+  </si>
+  <si>
+    <t>Quoc Nghia</t>
+  </si>
+  <si>
+    <t>T01</t>
+  </si>
+  <si>
+    <t>T02</t>
+  </si>
+  <si>
+    <t>T03</t>
+  </si>
+  <si>
+    <t>T04</t>
+  </si>
+  <si>
+    <t>T05</t>
+  </si>
+  <si>
+    <t>T06</t>
+  </si>
+  <si>
+    <t>T07</t>
+  </si>
+  <si>
+    <t>type_id</t>
+  </si>
+  <si>
+    <t>author_id</t>
+  </si>
+  <si>
+    <t>T08</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Author</t>
   </si>
 </sst>
 </file>
@@ -682,9 +685,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -999,573 +1000,573 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="71.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,3),"Minh Chánh","Phát Đạt","Quốc Nghĩa")</f>
-        <v>Phát Đạt</v>
+        <f ca="1">CHOOSE(RANDBETWEEN(1,2),"U01","U03",)</f>
+        <v>U03</v>
       </c>
       <c r="H2" s="6">
         <f ca="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44579</v>
+        <v>44607</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="71.25">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G3" s="1" t="str">
-        <f t="shared" ref="G3:G21" ca="1" si="0">CHOOSE(RANDBETWEEN(1,3),"Minh Chánh","Phát Đạt","Quốc Nghĩa")</f>
-        <v>Minh Chánh</v>
+        <f t="shared" ref="G3:G21" ca="1" si="0">CHOOSE(RANDBETWEEN(1,2),"U01","U03",)</f>
+        <v>U03</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" ref="H3:H21" ca="1" si="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44604</v>
+        <v>44676</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="199.5">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U03</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44690</v>
+        <v>44736</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="85.5">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U01</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44665</v>
+        <v>44730</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="85.5">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U03</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="313.5">
+        <v>44741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="327.75">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>U01</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44613</v>
+        <v>44686</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="162" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U03</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44583</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="242.25">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>U01</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44710</v>
+        <v>44708</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="213.75">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>U01</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44563</v>
+        <v>44616</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="171">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U03</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44682</v>
+        <v>44633</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="213.75">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>U01</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44733</v>
+        <v>44638</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="256.5">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>U03</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44674</v>
+        <v>44731</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="256.5">
       <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U03</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44592</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="213.75">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U03</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44684</v>
+        <v>44689</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="242.25">
       <c r="A16" s="1" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U03</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44717</v>
+        <v>44625</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="228">
       <c r="A17" s="1" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>U03</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44719</v>
+        <v>44650</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="165">
       <c r="A18" s="1" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>U01</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44733</v>
+        <v>44665</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="185.25">
       <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="G19" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Quốc Nghĩa</v>
+        <v>U01</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44563</v>
+        <v>44601</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="270.75">
       <c r="A20" s="1" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Minh Chánh</v>
+        <v>U03</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44652</v>
+        <v>44725</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="228">
       <c r="A21" s="1" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Phát Đạt</v>
+        <v>U01</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>44607</v>
+        <v>44698</v>
       </c>
     </row>
   </sheetData>
@@ -1577,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E6E3C9-52CD-4A4E-83C5-D2EDA47FC82E}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1602,86 +1603,98 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C2" s="8">
         <f ca="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44685</v>
+        <v>44583</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C3" s="8">
-        <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44658</v>
+        <f t="shared" ref="C3:C9" ca="1" si="0">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
+        <v>44641</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44567</v>
+        <v>44700</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="7" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44627</v>
+        <v>44694</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>142</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44698</v>
+        <v>44634</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="7" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44595</v>
+        <v>44706</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>30</v>
+        <v>144</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44566</v>
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>44737</v>
       </c>
     </row>
   </sheetData>
@@ -1691,42 +1704,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D48DC91-4CDE-46AB-9054-37BF0DD0F1D6}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5458866-346D-4D8E-9E2A-A3385C004668}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="7"/>
-    <col min="2" max="2" width="19.875" style="7" customWidth="1"/>
-    <col min="3" max="4" width="16.75" style="7" customWidth="1"/>
-    <col min="5" max="6" width="36.25" style="7" customWidth="1"/>
-    <col min="7" max="7" width="28" style="7" customWidth="1"/>
-    <col min="8" max="8" width="17.625" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="7"/>
+    <col min="1" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="7" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>7</v>
@@ -1736,138 +1746,75 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="7">
-        <v>123456789</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7">
-        <v>327147654</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="8">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="9">
         <f ca="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44627</v>
+        <v>44705</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="7">
-        <v>123456789</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7">
-        <v>327147654</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H6" ca="1" si="0">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
-        <v>44726</v>
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="9">
+        <f t="shared" ref="H3:H5" ca="1" si="0">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
+        <v>44718</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="7">
-        <v>123456789</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="7">
-        <v>327147654</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>44599</v>
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>44581</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="7">
-        <v>123456789</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="7">
-        <v>327147654</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>44634</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="7">
-        <v>123456789</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="7">
-        <v>327147654</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>44743</v>
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>44637</v>
       </c>
     </row>
   </sheetData>
@@ -1877,45 +1824,97 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5458866-346D-4D8E-9E2A-A3385C004668}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A4CD13-0212-4887-A73A-E7E25EC7FEBF}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="8" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>57</v>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="9">
+        <f ca="1">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
+        <v>44631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D5" ca="1" si="0">RANDBETWEEN(DATE(2022,1,1),DATE(2022,6,31))</f>
+        <v>44626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>5</v>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>44674</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>44636</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>